<commit_message>
Initial cut on parsing sharedStrings.xml part.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -374,15 +395,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,60 +411,111 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="E11">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="F12">
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="G13">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="H14">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="I15">
+        <v>66.599999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle format runs in shared string record.
For now I'll ignore the format attributes.  I'll take care of that
later.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Unformatted" sheetId="1" r:id="rId1"/>
+    <sheet name="Simple Format" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -64,14 +64,110 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>Bold</t>
+  </si>
+  <si>
+    <t>Italic</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Part </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and part </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>italic</t>
+    </r>
+  </si>
+  <si>
+    <t>Same Text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Same</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Text</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,8 +195,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,13 +623,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Pick up font size.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,74 @@
         <scheme val="minor"/>
       </rPr>
       <t>Text</t>
+    </r>
+  </si>
+  <si>
+    <t>Big font</t>
+  </si>
+  <si>
+    <t>Medium font</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="72"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Big</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="36"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>medium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>small</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fonts.</t>
     </r>
   </si>
 </sst>
@@ -150,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +237,27 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -195,10 +284,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,10 +714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,6 +749,21 @@
       </c>
       <c r="D2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="92.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="46.5">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.25">
+      <c r="A6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pick up font names too.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -211,6 +211,85 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> fonts.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Calibri </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tahoma</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Times</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="28"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>oman</t>
     </r>
   </si>
 </sst>
@@ -218,7 +297,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +341,37 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -714,10 +824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -764,6 +874,11 @@
     <row r="6" spans="1:4" ht="92.25">
       <c r="A6" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="35.25">
+      <c r="A7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pick up and store border styles.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,30 @@
       </rPr>
       <t>oman</t>
     </r>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>outline</t>
+  </si>
+  <si>
+    <t>Borders</t>
+  </si>
+  <si>
+    <t>Fills</t>
   </si>
 </sst>
 </file>
@@ -374,15 +398,20 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray0625">
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -390,16 +419,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,10 +911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -836,7 +923,7 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -847,7 +934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -861,25 +948,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="92.25">
+    <row r="4" spans="1:6" ht="92.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="46.5">
+    <row r="5" spans="1:6" ht="46.5">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="92.25">
+    <row r="6" spans="1:6" ht="92.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="35.25">
+    <row r="7" spans="1:6" ht="35.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pick up fill colors and apply them to html output.
The colors are still hard-coded.  I still need to convert RGB text
into values properly.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -314,7 +314,7 @@
     <t>Borders</t>
   </si>
   <si>
-    <t>Fills</t>
+    <t>Background colors</t>
   </si>
 </sst>
 </file>
@@ -406,8 +406,9 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="gray0625">
-        <bgColor rgb="FFFF0000"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -914,7 +915,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Finally process RGB colors for fill attributes correctly.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -398,7 +398,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +408,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -488,6 +512,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,7 +943,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1001,6 +1029,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a new sheet to import formula cells.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Unformatted" sheetId="1" r:id="rId1"/>
     <sheet name="Simple Format" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Formula" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -942,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1042,12 +1042,200 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1">
+        <f>SUM(Unformatted!B2:B8)</f>
+        <v>28</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <f>D1*10</f>
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <f>SUM(D1:E1)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <f>A1*2</f>
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E13" si="0">D2*10</f>
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F13" si="1">SUM(D2:E2)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <f>SUM(A1:A2)</f>
+        <v>84</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="G13">
+        <f>SUM(E13:F13)</f>
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>